<commit_message>
added 2003 india plots
</commit_message>
<xml_diff>
--- a/data/MASTER_FILE_SCALED_2003-13.xlsx
+++ b/data/MASTER_FILE_SCALED_2003-13.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="8295" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="8295"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -652,9 +652,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BD2" sqref="BD2:BD36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F2" sqref="F2:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +662,7 @@
     <col min="1" max="1" width="23.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="2" customWidth="1"/>
     <col min="7" max="9" width="16.85546875" style="2" customWidth="1"/>
@@ -709,7 +709,7 @@
     <col min="58" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7511,8 +7511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection sqref="A1:C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7527,8 +7527,8 @@
       <c r="B1" t="s">
         <v>84</v>
       </c>
-      <c r="C1">
-        <v>58</v>
+      <c r="C1" s="2">
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -7538,8 +7538,8 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>4241</v>
+      <c r="C2" s="2">
+        <v>4608</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -7549,9 +7549,7 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>11</v>
-      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -7560,8 +7558,8 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>2950</v>
+      <c r="C4" s="2">
+        <v>3035</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -7571,8 +7569,8 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
-        <v>3935</v>
+      <c r="C5" s="2">
+        <v>4613</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -7582,8 +7580,8 @@
       <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="C6">
-        <v>212</v>
+      <c r="C6" s="2">
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -7593,8 +7591,8 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7">
-        <v>6112</v>
+      <c r="C7" s="2">
+        <v>4417</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7604,7 +7602,7 @@
       <c r="B8" t="s">
         <v>85</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>0</v>
       </c>
     </row>
@@ -7615,8 +7613,8 @@
       <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c r="C9">
-        <v>18</v>
+      <c r="C9" s="2">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -7626,8 +7624,8 @@
       <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="C10">
-        <v>2935</v>
+      <c r="C10" s="2">
+        <v>1913</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -7637,8 +7635,8 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>107</v>
+      <c r="C11" s="2">
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -7648,8 +7646,8 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>3284</v>
+      <c r="C12" s="2">
+        <v>2820</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -7659,8 +7657,8 @@
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13">
-        <v>6313</v>
+      <c r="C13" s="2">
+        <v>3574</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -7670,8 +7668,8 @@
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14">
-        <v>740</v>
+      <c r="C14" s="2">
+        <v>357</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -7681,8 +7679,8 @@
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15">
-        <v>278</v>
+      <c r="C15" s="2">
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -7692,8 +7690,8 @@
       <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16">
-        <v>3836</v>
+      <c r="C16" s="2">
+        <v>4110</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7703,8 +7701,8 @@
       <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17">
-        <v>4244</v>
+      <c r="C17" s="2">
+        <v>2428</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -7714,8 +7712,8 @@
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18">
-        <v>2289</v>
+      <c r="C18" s="2">
+        <v>1705</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -7725,7 +7723,7 @@
       <c r="B19" t="s">
         <v>35</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>0</v>
       </c>
     </row>
@@ -7736,8 +7734,8 @@
       <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20">
-        <v>15494</v>
+      <c r="C20" s="2">
+        <v>11139</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -7747,8 +7745,8 @@
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21">
-        <v>7315</v>
+      <c r="C21" s="2">
+        <v>6567</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -7758,8 +7756,8 @@
       <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="C22">
-        <v>34</v>
+      <c r="C22" s="2">
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -7769,8 +7767,8 @@
       <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C23">
-        <v>58</v>
+      <c r="C23" s="2">
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -7780,8 +7778,8 @@
       <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="C24">
-        <v>339</v>
+      <c r="C24" s="2">
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -7791,8 +7789,8 @@
       <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="C25">
-        <v>91</v>
+      <c r="C25" s="2">
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -7802,8 +7800,8 @@
       <c r="B26" t="s">
         <v>86</v>
       </c>
-      <c r="C26">
-        <v>3340</v>
+      <c r="C26" s="2">
+        <v>3130</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -7813,8 +7811,8 @@
       <c r="B27" t="s">
         <v>36</v>
       </c>
-      <c r="C27">
-        <v>5886</v>
+      <c r="C27" s="2">
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -7824,8 +7822,8 @@
       <c r="B28" t="s">
         <v>24</v>
       </c>
-      <c r="C28">
-        <v>87</v>
+      <c r="C28" s="2">
+        <v>2926</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -7835,8 +7833,8 @@
       <c r="B29" t="s">
         <v>25</v>
       </c>
-      <c r="C29">
-        <v>5319</v>
+      <c r="C29" s="2">
+        <v>5482</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -7846,8 +7844,8 @@
       <c r="B30" t="s">
         <v>26</v>
       </c>
-      <c r="C30">
-        <v>93</v>
+      <c r="C30" s="2">
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -7857,8 +7855,8 @@
       <c r="B31" t="s">
         <v>27</v>
       </c>
-      <c r="C31">
-        <v>4403</v>
+      <c r="C31" s="2">
+        <v>5754</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -7868,8 +7866,8 @@
       <c r="B32" t="s">
         <v>28</v>
       </c>
-      <c r="C32">
-        <v>498</v>
+      <c r="C32" s="2">
+        <v>488</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -7879,8 +7877,8 @@
       <c r="B33" t="s">
         <v>29</v>
       </c>
-      <c r="C33">
-        <v>23179</v>
+      <c r="C33" s="2">
+        <v>5376</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -7890,8 +7888,8 @@
       <c r="B34" t="s">
         <v>30</v>
       </c>
-      <c r="C34">
-        <v>1591</v>
+      <c r="C34" s="2">
+        <v>587</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -7901,8 +7899,8 @@
       <c r="B35" t="s">
         <v>31</v>
       </c>
-      <c r="C35">
-        <v>4388</v>
+      <c r="C35" s="2">
+        <v>2616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>